<commit_message>
added automatic job entry from excel files
</commit_message>
<xml_diff>
--- a/testdata/2023_clean/Helferliste_Infrastruktur.xlsx
+++ b/testdata/2023_clean/Helferliste_Infrastruktur.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t xml:space="preserve">Stustaculum 2023 - Helferliste</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Spezifizierung/Ort:</t>
   </si>
   <si>
-    <t xml:space="preserve">Manhattan</t>
+    <t xml:space="preserve">Infrastruktur</t>
   </si>
   <si>
     <t xml:space="preserve">Treffpunkt: Infozelt</t>
@@ -927,7 +927,7 @@
   <dimension ref="A1:L200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -958,7 +958,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1030,11 +1030,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17" t="s">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="17"/>
       <c r="C6" s="18" t="n">
         <v>45084</v>
       </c>
@@ -1057,8 +1057,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="n">
         <v>45085</v>
@@ -1088,8 +1090,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="21"/>
       <c r="C8" s="18" t="n">
         <v>45086</v>
@@ -1119,8 +1123,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" s="21"/>
       <c r="C9" s="18" t="n">
         <v>45087</v>
@@ -1419,6 +1425,9 @@
       <c r="E28" s="24"/>
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
+      <c r="K28" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>